<commit_message>
Add analyser to cash
Change-Id: I4c7fd5bb696d9116a1c6c97ec5fe8e800a9b6be3
</commit_message>
<xml_diff>
--- a/Doc/FinanceAnalysis_Tang.xlsx
+++ b/Doc/FinanceAnalysis_Tang.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8517B05-231E-4FDA-BAC7-92FA15094EF7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9460CD0E-58E1-45F4-BBA8-2423312E65BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="195">
   <si>
     <t>Table</t>
   </si>
@@ -109,9 +109,6 @@
     <t>货币资金充裕却有很多有息甚至高息负债</t>
   </si>
   <si>
-    <t>定期存款很多，其它货币资金很多，流动资严重缺乏</t>
-  </si>
-  <si>
     <t>其它货币资金数额巨大但没有合理解释</t>
   </si>
   <si>
@@ -602,6 +599,18 @@
   </si>
   <si>
     <t>T001</t>
+  </si>
+  <si>
+    <t>T002</t>
+  </si>
+  <si>
+    <t>定期存款很多，其它货币资金很多，流动资金严重缺乏</t>
+  </si>
+  <si>
+    <t>ts没有此数据</t>
+  </si>
+  <si>
+    <t>流动资金指什么</t>
   </si>
 </sst>
 </file>
@@ -923,9 +932,9 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,7 +949,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -949,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -964,76 +973,91 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
       <c r="E7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="F10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1041,7 +1065,7 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1049,7 +1073,7 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1057,15 +1081,15 @@
         <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
@@ -1073,7 +1097,7 @@
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
@@ -1081,10 +1105,10 @@
         <v>22</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
@@ -1092,75 +1116,75 @@
         <v>23</v>
       </c>
       <c r="F19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" t="s">
         <v>30</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.3">
@@ -1171,18 +1195,18 @@
         <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>15</v>
       </c>
@@ -1190,250 +1214,256 @@
         <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F36" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F37" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
         <v>39</v>
       </c>
-      <c r="F39" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
+      <c r="E41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
         <v>41</v>
       </c>
-      <c r="F41" t="s">
+      <c r="E43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F43" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
+      <c r="F45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="E46" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="F46" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>191</v>
+      </c>
       <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F48" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>191</v>
+      </c>
       <c r="E49" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F52" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E53" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F53" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>70</v>
       </c>
-      <c r="F54" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E57" s="1" t="s">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E58" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E58" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
+        <v>72</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" t="s">
         <v>74</v>
       </c>
-      <c r="F60" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F62" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
+      <c r="E63" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
+        <v>88</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="F67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
+        <v>86</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
+        <v>82</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
+        <v>107</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="F73" t="s">
         <v>109</v>
-      </c>
-      <c r="F73" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
+        <v>100</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F74" t="s">
         <v>101</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F74" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
+        <v>102</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="F75" t="s">
         <v>104</v>
-      </c>
-      <c r="F75" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E76" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F76" t="s">
         <v>106</v>
-      </c>
-      <c r="F76" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.3">
@@ -1441,310 +1471,339 @@
         <v>5</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
+        <v>90</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="F79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E80" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E81" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
+        <v>169</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E84" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="F84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E85" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F87" t="s">
         <v>111</v>
-      </c>
-      <c r="F87" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E88" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F88" t="s">
         <v>113</v>
-      </c>
-      <c r="F88" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E89" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F89" t="s">
         <v>115</v>
-      </c>
-      <c r="F89" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E90" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F90" t="s">
         <v>117</v>
-      </c>
-      <c r="F90" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E91" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F91" t="s">
         <v>153</v>
-      </c>
-      <c r="F91" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E92" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F92" t="s">
         <v>168</v>
-      </c>
-      <c r="F92" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E93" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F93" t="s">
         <v>155</v>
-      </c>
-      <c r="F93" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E94" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
+        <v>119</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="F96" t="s">
         <v>121</v>
-      </c>
-      <c r="F96" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E97" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
+        <v>122</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F100" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E101" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F101" t="s">
         <v>125</v>
-      </c>
-      <c r="F101" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E102" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F102" t="s">
         <v>128</v>
-      </c>
-      <c r="F102" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E103" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F103" t="s">
         <v>157</v>
-      </c>
-      <c r="F103" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="104" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E104" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F104" t="s">
         <v>159</v>
-      </c>
-      <c r="F104" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="106" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C106" t="s">
+        <v>129</v>
+      </c>
+      <c r="E106" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C108" t="s">
+        <v>160</v>
+      </c>
+      <c r="E108" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="F108" t="s">
         <v>162</v>
-      </c>
-      <c r="F108" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D109" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F109" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D110" t="s">
+        <v>165</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F110" t="s">
         <v>166</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F110" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
+        <v>131</v>
+      </c>
+      <c r="E112" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C113" t="s">
+        <v>133</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C115" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>190</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E116" s="1" t="s">
+      <c r="F116" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>190</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F117" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E117" s="1" t="s">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>190</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F117" t="s">
+      <c r="F118" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>190</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F119" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>190</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F121" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>190</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F122" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>190</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F123" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>190</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F124" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E118" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F118" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E119" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F119" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E121" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F121" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E122" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F122" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E123" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F123" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E124" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F124" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -1754,40 +1813,40 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C127" t="s">
+        <v>45</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C128" t="s">
+        <v>61</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="F128" t="s">
         <v>63</v>
-      </c>
-      <c r="F128" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="129" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C129" t="s">
+        <v>64</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="130" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
+        <v>57</v>
+      </c>
+      <c r="E130" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E130" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F130" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="132" spans="3:6" x14ac:dyDescent="0.3">
@@ -1811,34 +1870,34 @@
     </row>
     <row r="134" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C134" t="s">
+        <v>75</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="135" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C135" t="s">
+        <v>77</v>
+      </c>
+      <c r="E135" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="136" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C136" t="s">
+        <v>55</v>
+      </c>
+      <c r="E136" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="137" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C137" t="s">
+        <v>59</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add analyzer to asets
Change-Id: Ide3bb3e49ef6c9ebaecee2c75bcf99cbbb236440
</commit_message>
<xml_diff>
--- a/Doc/FinanceAnalysis_Tang.xlsx
+++ b/Doc/FinanceAnalysis_Tang.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A748A465-F576-4A72-89CB-A49DCD839A06}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D791548-E6ED-4F33-A09F-729B3AEDFA39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="203">
   <si>
     <t>Table</t>
   </si>
@@ -612,12 +612,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>其他应付款</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>预付账款占营业收入或营业成本的比例大幅波动</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T004</t>
+  </si>
+  <si>
+    <t>其他应付款</t>
+  </si>
+  <si>
+    <t>ts无此科目</t>
+  </si>
+  <si>
+    <t>难以自动判定</t>
+  </si>
+  <si>
+    <t>T004 - 仅固定资产</t>
+  </si>
+  <si>
+    <t>T005</t>
   </si>
 </sst>
 </file>
@@ -946,9 +960,9 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1207,7 +1221,7 @@
         <v>188</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F25" t="s">
         <v>172</v>
@@ -1215,7 +1229,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="C27" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>63</v>
@@ -1252,6 +1266,9 @@
       </c>
     </row>
     <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>191</v>
+      </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
@@ -1263,6 +1280,9 @@
       </c>
     </row>
     <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>201</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>45</v>
       </c>
@@ -1271,6 +1291,9 @@
       </c>
     </row>
     <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>199</v>
+      </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
@@ -1282,6 +1305,9 @@
       </c>
     </row>
     <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>191</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>13</v>
       </c>
@@ -1290,6 +1316,9 @@
       </c>
     </row>
     <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>197</v>
+      </c>
       <c r="C39" t="s">
         <v>33</v>
       </c>
@@ -1301,6 +1330,9 @@
       </c>
     </row>
     <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>197</v>
+      </c>
       <c r="C41" t="s">
         <v>35</v>
       </c>
@@ -1312,6 +1344,9 @@
       </c>
     </row>
     <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>191</v>
+      </c>
       <c r="C43" t="s">
         <v>39</v>
       </c>
@@ -1323,6 +1358,9 @@
       </c>
     </row>
     <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>191</v>
+      </c>
       <c r="E44" s="1" t="s">
         <v>40</v>
       </c>
@@ -1352,12 +1390,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="1:6">
       <c r="C49" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>200</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>47</v>
       </c>
@@ -1365,7 +1406,10 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>201</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>48</v>
       </c>
@@ -1373,7 +1417,10 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>200</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>65</v>
       </c>
@@ -1381,12 +1428,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="1:6">
       <c r="B54" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="1:6">
       <c r="C55" t="s">
         <v>93</v>
       </c>
@@ -1394,12 +1441,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="1:6">
       <c r="E56" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="1:6">
       <c r="C58" t="s">
         <v>68</v>
       </c>
@@ -1410,7 +1457,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>202</v>
+      </c>
       <c r="C60" t="s">
         <v>75</v>
       </c>
@@ -1421,7 +1471,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>202</v>
+      </c>
       <c r="C61" t="s">
         <v>76</v>
       </c>
@@ -1432,7 +1485,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="1:6">
       <c r="C63" t="s">
         <v>80</v>
       </c>
@@ -1440,7 +1493,10 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="3:6">
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>202</v>
+      </c>
       <c r="C65" t="s">
         <v>84</v>
       </c>
@@ -1451,7 +1507,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="3:6">
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>202</v>
+      </c>
       <c r="C67" t="s">
         <v>82</v>
       </c>
@@ -1459,7 +1518,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="3:6">
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>202</v>
+      </c>
       <c r="C69" t="s">
         <v>78</v>
       </c>
@@ -1470,7 +1532,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="3:6">
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>202</v>
+      </c>
       <c r="C71" t="s">
         <v>103</v>
       </c>
@@ -1481,7 +1546,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="72" spans="3:6">
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>202</v>
+      </c>
       <c r="C72" t="s">
         <v>96</v>
       </c>
@@ -1492,7 +1560,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="3:6">
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>202</v>
+      </c>
       <c r="C73" t="s">
         <v>98</v>
       </c>
@@ -1503,7 +1574,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="3:6">
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>202</v>
+      </c>
       <c r="E74" s="1" t="s">
         <v>101</v>
       </c>
@@ -1511,7 +1585,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="3:6">
+    <row r="76" spans="1:6">
       <c r="C76" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1593,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="3:6">
+    <row r="77" spans="1:6">
       <c r="D77" t="s">
         <v>86</v>
       </c>
@@ -1530,7 +1604,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="3:6">
+    <row r="78" spans="1:6">
       <c r="E78" s="1" t="s">
         <v>88</v>
       </c>
@@ -1538,7 +1612,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="3:6">
+    <row r="79" spans="1:6">
       <c r="E79" s="1" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Add analyzer for income
Change-Id: I6e5b895f3d7d73dab22ff1dd61578e8690e95b1a
</commit_message>
<xml_diff>
--- a/Doc/FinanceAnalysis_Tang.xlsx
+++ b/Doc/FinanceAnalysis_Tang.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D206FA-ABBF-4365-A97D-B8B85C8C7535}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCF15C3-5B8F-47BC-9484-4C3434B1DA99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,9 +963,9 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>